<commit_message>
ISTTT 23 first submit
</commit_message>
<xml_diff>
--- a/Example1/Data.xlsx
+++ b/Example1/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241F16F0-3FB2-4B42-BCF0-60F74593286F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599160C3-B499-4DA8-8D28-CF82E8CDEA49}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,8 @@
     <sheet name="Para" sheetId="2" r:id="rId3"/>
     <sheet name="PasWeight" sheetId="3" r:id="rId4"/>
     <sheet name="JndAbs" sheetId="4" r:id="rId5"/>
-    <sheet name="JndPer" sheetId="5" r:id="rId6"/>
+    <sheet name="ComputeWeighting" sheetId="9" r:id="rId6"/>
+    <sheet name="JndPer" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Fare</t>
   </si>
@@ -88,7 +89,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +100,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -113,12 +129,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +603,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -562,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -579,7 +664,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -596,7 +681,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -618,7 +703,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,7 +732,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -716,7 +801,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +884,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,10 +913,10 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="C3">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -873,10 +958,703 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040823F6-5E10-4BE6-B866-7289121CDB0B}">
+  <dimension ref="F4:W43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>70</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f>I5*0.2</f>
+        <v>14</v>
+      </c>
+      <c r="L5">
+        <f>-1*J5</f>
+        <v>-3</v>
+      </c>
+      <c r="M5">
+        <f>H5+K5+L5</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>96</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K8" si="0">I6*0.2</f>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L8" si="1">-1*J6</f>
+        <v>-4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M8" si="2">H6+K6+L6</f>
+        <v>23.200000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>75</v>
+      </c>
+      <c r="J7" s="3">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>105</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>7</v>
+      </c>
+      <c r="M17">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>70</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>-3</v>
+      </c>
+      <c r="L18">
+        <v>12</v>
+      </c>
+      <c r="M18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>96</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>12</v>
+      </c>
+      <c r="K19" s="2">
+        <v>70</v>
+      </c>
+      <c r="L19">
+        <v>16</v>
+      </c>
+      <c r="M19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>75</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>8</v>
+      </c>
+      <c r="K20" s="4">
+        <v>96</v>
+      </c>
+      <c r="R20">
+        <v>12</v>
+      </c>
+      <c r="S20">
+        <v>70</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>-3</v>
+      </c>
+      <c r="W20">
+        <f>R20+0.2*S20+V20</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>105</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>10</v>
+      </c>
+      <c r="K21" s="4">
+        <v>75</v>
+      </c>
+      <c r="R21">
+        <v>8</v>
+      </c>
+      <c r="S21">
+        <v>96</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>-4</v>
+      </c>
+      <c r="W21">
+        <f t="shared" ref="W21:W23" si="3">R21+0.2*S21+V21</f>
+        <v>23.200000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J22" s="3">
+        <v>15</v>
+      </c>
+      <c r="K22" s="4">
+        <v>105</v>
+      </c>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="S22">
+        <v>75</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>-4</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <v>15</v>
+      </c>
+      <c r="S23">
+        <v>105</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>-2</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F29" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G29" s="5">
+        <f>0.6*0.2</f>
+        <v>0.12</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F30" s="5">
+        <f>PathCost!A2</f>
+        <v>12</v>
+      </c>
+      <c r="G30" s="5">
+        <f>PathCost!B2</f>
+        <v>70</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <f>PathCost!E2</f>
+        <v>-3</v>
+      </c>
+      <c r="K30" s="5">
+        <f>F30*$F$29</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="L30" s="5">
+        <f>$G$29*G30</f>
+        <v>8.4</v>
+      </c>
+      <c r="M30" s="5">
+        <f>J30*$J$29</f>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="N30" s="6">
+        <f>K30+L30+M30</f>
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="P30">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="31" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F31" s="5">
+        <f>PathCost!A3</f>
+        <v>8</v>
+      </c>
+      <c r="G31" s="5">
+        <f>PathCost!B3</f>
+        <v>96</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <f>PathCost!E3</f>
+        <v>-4</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" ref="K31:K33" si="4">F31*$F$29</f>
+        <v>0.8</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" ref="L31:L33" si="5">$G$29*G31</f>
+        <v>11.52</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" ref="M31:M33" si="6">J31*$J$29</f>
+        <v>-1.2</v>
+      </c>
+      <c r="N31" s="6">
+        <f t="shared" ref="N31:N33" si="7">K31+L31+M31</f>
+        <v>11.120000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F32" s="5">
+        <f>PathCost!A4</f>
+        <v>10</v>
+      </c>
+      <c r="G32" s="5">
+        <f>PathCost!B4</f>
+        <v>75</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <f>PathCost!E4</f>
+        <v>-4</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" si="6"/>
+        <v>-1.2</v>
+      </c>
+      <c r="N32" s="6">
+        <f t="shared" si="7"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F33" s="5">
+        <f>PathCost!A5</f>
+        <v>15</v>
+      </c>
+      <c r="G33" s="5">
+        <f>PathCost!B5</f>
+        <v>105</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
+        <f>PathCost!E5</f>
+        <v>-2</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="5"/>
+        <v>12.6</v>
+      </c>
+      <c r="M33" s="5">
+        <f t="shared" si="6"/>
+        <v>-0.6</v>
+      </c>
+      <c r="N33" s="6">
+        <f t="shared" si="7"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+    </row>
+    <row r="39" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F39" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G39" s="5">
+        <f>0.3*0.2</f>
+        <v>0.06</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+    </row>
+    <row r="40" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F40" s="5">
+        <f>F30</f>
+        <v>12</v>
+      </c>
+      <c r="G40" s="5">
+        <f>PathCost!B2</f>
+        <v>70</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
+        <f>J30</f>
+        <v>-3</v>
+      </c>
+      <c r="K40" s="5">
+        <f>F40*$F$39</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="L40" s="5">
+        <f>$G$39*G40</f>
+        <v>4.2</v>
+      </c>
+      <c r="M40" s="5">
+        <f>J40*$J$39</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="N40" s="6">
+        <f>K40+L40+M40</f>
+        <v>11.099999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F41" s="5">
+        <f t="shared" ref="F41:F43" si="8">F31</f>
+        <v>8</v>
+      </c>
+      <c r="G41" s="5">
+        <f>PathCost!B3</f>
+        <v>96</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" ref="J41:J43" si="9">J31</f>
+        <v>-4</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" ref="K41:K43" si="10">F41*$F$39</f>
+        <v>4.8</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" ref="L41:L43" si="11">$G$39*G41</f>
+        <v>5.76</v>
+      </c>
+      <c r="M41" s="5">
+        <f t="shared" ref="M41:M43" si="12">J41*$J$39</f>
+        <v>-0.4</v>
+      </c>
+      <c r="N41" s="6">
+        <f t="shared" ref="N41:N43" si="13">K41+L41+M41</f>
+        <v>10.159999999999998</v>
+      </c>
+      <c r="P41">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="42" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F42" s="5">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="G42" s="5">
+        <f>PathCost!B4</f>
+        <v>75</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="L42" s="5">
+        <f t="shared" si="11"/>
+        <v>4.5</v>
+      </c>
+      <c r="M42" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.4</v>
+      </c>
+      <c r="N42" s="6">
+        <f t="shared" si="13"/>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F43" s="5">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="G43" s="5">
+        <f>PathCost!B5</f>
+        <v>105</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" si="11"/>
+        <v>6.3</v>
+      </c>
+      <c r="M43" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.2</v>
+      </c>
+      <c r="N43" s="6">
+        <f t="shared" si="13"/>
+        <v>15.100000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F28:N28"/>
+    <mergeCell ref="F38:N38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5273FBB7-1D0C-410B-A9BB-B365110DD13A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first multi weight version
</commit_message>
<xml_diff>
--- a/Example1/Data.xlsx
+++ b/Example1/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599160C3-B499-4DA8-8D28-CF82E8CDEA49}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8FF13789-CE33-4C26-98D4-0E9D08E34C80}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="9660" tabRatio="901" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PathCost (2)" sheetId="7" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="Para" sheetId="2" r:id="rId3"/>
     <sheet name="PasWeight" sheetId="3" r:id="rId4"/>
     <sheet name="JndAbs" sheetId="4" r:id="rId5"/>
-    <sheet name="ComputeWeighting" sheetId="9" r:id="rId6"/>
-    <sheet name="JndPer" sheetId="5" r:id="rId7"/>
+    <sheet name="CheckWeighting" sheetId="9" r:id="rId6"/>
+    <sheet name="default_Jnd" sheetId="10" r:id="rId7"/>
+    <sheet name="JndPer" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>Fare</t>
   </si>
@@ -83,6 +84,18 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Abs</t>
+  </si>
+  <si>
+    <t>Per</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
 </sst>
 </file>
@@ -490,9 +503,9 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -530,7 +543,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -551,7 +564,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -572,7 +585,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -606,9 +619,9 @@
       <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -642,7 +655,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -659,7 +672,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -676,7 +689,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -703,15 +716,15 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -719,7 +732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -727,7 +740,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -735,7 +748,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -743,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -751,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -759,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -767,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -775,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -783,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -801,17 +814,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -819,7 +832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -830,7 +843,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -841,7 +854,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -852,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -863,7 +876,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -884,12 +897,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -897,7 +910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -908,7 +921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -919,7 +932,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -930,7 +943,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -941,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -961,14 +974,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040823F6-5E10-4BE6-B866-7289121CDB0B}">
   <dimension ref="F4:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:X57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5">
         <v>12</v>
       </c>
@@ -991,7 +1004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H6">
         <v>8</v>
       </c>
@@ -1014,7 +1027,7 @@
         <v>23.200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H7">
         <v>10</v>
       </c>
@@ -1037,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H8">
         <v>15</v>
       </c>
@@ -1060,8 +1073,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P12" s="1">
         <v>12</v>
       </c>
@@ -1069,7 +1082,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P13" s="3">
         <v>8</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="3">
         <v>10</v>
       </c>
@@ -1085,7 +1098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P15" s="3">
         <v>15</v>
       </c>
@@ -1093,7 +1106,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="8:17" x14ac:dyDescent="0.25">
       <c r="L16">
         <v>14</v>
       </c>
@@ -1101,7 +1114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:23" x14ac:dyDescent="0.25">
       <c r="L17">
         <v>7</v>
       </c>
@@ -1109,7 +1122,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>12</v>
       </c>
@@ -1132,7 +1145,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>8</v>
       </c>
@@ -1158,7 +1171,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>10</v>
       </c>
@@ -1197,7 +1210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>15</v>
       </c>
@@ -1236,7 +1249,7 @@
         <v>23.200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="6:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J22" s="3">
         <v>15</v>
       </c>
@@ -1263,7 +1276,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:23" x14ac:dyDescent="0.25">
       <c r="R23">
         <v>15</v>
       </c>
@@ -1284,7 +1297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F28" s="7" t="s">
         <v>18</v>
       </c>
@@ -1297,7 +1310,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F29" s="5">
         <v>0.1</v>
       </c>
@@ -1315,7 +1328,7 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F30" s="5">
         <f>PathCost!A2</f>
         <v>12</v>
@@ -1354,7 +1367,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="31" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F31" s="5">
         <f>PathCost!A3</f>
         <v>8</v>
@@ -1390,7 +1403,7 @@
         <v>11.120000000000001</v>
       </c>
     </row>
-    <row r="32" spans="6:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F32" s="5">
         <f>PathCost!A4</f>
         <v>10</v>
@@ -1426,7 +1439,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F33" s="5">
         <f>PathCost!A5</f>
         <v>15</v>
@@ -1462,7 +1475,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F38" s="7" t="s">
         <v>17</v>
       </c>
@@ -1475,7 +1488,7 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F39" s="5">
         <v>0.6</v>
       </c>
@@ -1493,7 +1506,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F40" s="5">
         <f>F30</f>
         <v>12</v>
@@ -1529,7 +1542,7 @@
         <v>11.099999999999998</v>
       </c>
     </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F41" s="5">
         <f t="shared" ref="F41:F43" si="8">F31</f>
         <v>8</v>
@@ -1568,7 +1581,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F42" s="5">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -1604,7 +1617,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F43" s="5">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -1646,11 +1659,125 @@
     <mergeCell ref="F38:N38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ACB963-64CE-4B19-B75F-D0360E909A6C}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5273FBB7-1D0C-410B-A9BB-B365110DD13A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1658,9 +1785,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1806,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +1817,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1701,7 +1828,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1712,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>

</xml_diff>